<commit_message>
feat: Update product DTO and interface to use number types for cost and dimensions
</commit_message>
<xml_diff>
--- a/src/assets/files/InvalidProduct.xlsx
+++ b/src/assets/files/InvalidProduct.xlsx
@@ -460,13 +460,13 @@
         <v>[object Object]</v>
       </c>
       <c r="B2" t="str">
-        <v>SP001</v>
+        <v>SP0012</v>
       </c>
       <c r="C2" t="str">
-        <v>SKU001</v>
+        <v>SKU0012</v>
       </c>
       <c r="D2" t="str">
-        <v>Sản phẩm mẫu</v>
+        <v>Sản phẩm mẫu1</v>
       </c>
       <c r="E2" t="str">
         <v>Tre đan</v>
@@ -477,8 +477,8 @@
       <c r="G2" t="str">
         <v>Cái</v>
       </c>
-      <c r="H2" t="str">
-        <v>"10000"</v>
+      <c r="H2">
+        <v>10000</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
feat(cors): configure CORS settings for enhanced security and flexibility
</commit_message>
<xml_diff>
--- a/src/assets/files/InvalidProduct.xlsx
+++ b/src/assets/files/InvalidProduct.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <r>
       <rPr>
@@ -135,40 +135,7 @@
     <t>Nội dung lỗi</t>
   </si>
   <si>
-    <t>SP001</t>
-  </si>
-  <si>
-    <t>SKU001</t>
-  </si>
-  <si>
-    <t>Sản phẩm mẫu</t>
-  </si>
-  <si>
-    <t>Tre đan</t>
-  </si>
-  <si>
-    <t>Quai rộng, phủ sơn bóng</t>
-  </si>
-  <si>
-    <t>Cái</t>
-  </si>
-  <si>
-    <t>Ghi chú mẫu</t>
-  </si>
-  <si>
-    <t>8934567890123</t>
-  </si>
-  <si>
-    <t>4602.99</t>
-  </si>
-  <si>
-    <t>Việt Nam</t>
-  </si>
-  <si>
-    <t>https://example.com/image.jpg</t>
-  </si>
-  <si>
-    <t>Mã sản phẩm đã tồn tại trong hệ thống, SKU đã tồn tại trong hệ thống, Barcode đã tồn tại trong hệ thống, HSCode đã tồn tại trong hệ thống.</t>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -231,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -240,9 +207,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -596,16 +560,14 @@
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="12" width="14" customWidth="1"/>
+    <col min="8" max="12" width="14" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
     <col min="14" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="31" customWidth="1"/>
-    <col min="18" max="18" width="140" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
+    <col min="18" max="18" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="24" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -668,56 +630,8 @@
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="4">
-        <v>10000</v>
-      </c>
-      <c r="H2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="N2" s="4">
-        <v>20</v>
-      </c>
-      <c r="O2" s="4">
-        <v>10</v>
-      </c>
-      <c r="P2" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="R2" s="3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>